<commit_message>
bug fixes in count pipeline and updated counting data
</commit_message>
<xml_diff>
--- a/rgb/data/weighted_count_data_v2.xlsx
+++ b/rgb/data/weighted_count_data_v2.xlsx
@@ -757,7 +757,7 @@
         <v>158</v>
       </c>
       <c r="C18" t="n">
-        <v>24692</v>
+        <v>16120</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -829,10 +829,10 @@
         <v>292</v>
       </c>
       <c r="C22" t="n">
-        <v>67072</v>
+        <v>53130</v>
       </c>
       <c r="D22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame00173_id292.png", "frame00173_id292.png")</f>
@@ -2413,7 +2413,7 @@
         <v>1585</v>
       </c>
       <c r="C110" t="n">
-        <v>56166</v>
+        <v>52614</v>
       </c>
       <c r="D110" t="n">
         <v>1</v>
@@ -3439,10 +3439,10 @@
         <v>2532</v>
       </c>
       <c r="C167" t="n">
-        <v>72274</v>
+        <v>46494</v>
       </c>
       <c r="D167" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E167">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame00984_id2532.png", "frame00984_id2532.png")</f>
@@ -5509,7 +5509,7 @@
         <v>4453</v>
       </c>
       <c r="C282" t="n">
-        <v>70900</v>
+        <v>68094</v>
       </c>
       <c r="D282" t="n">
         <v>2</v>
@@ -5833,7 +5833,7 @@
         <v>4633</v>
       </c>
       <c r="C300" t="n">
-        <v>39740</v>
+        <v>21140</v>
       </c>
       <c r="D300" t="n">
         <v>1</v>
@@ -6679,7 +6679,7 @@
         <v>5322</v>
       </c>
       <c r="C347" t="n">
-        <v>88214</v>
+        <v>82348</v>
       </c>
       <c r="D347" t="n">
         <v>2</v>
@@ -6787,7 +6787,7 @@
         <v>5482</v>
       </c>
       <c r="C353" t="n">
-        <v>85762</v>
+        <v>71370</v>
       </c>
       <c r="D353" t="n">
         <v>2</v>
@@ -7651,7 +7651,7 @@
         <v>6108</v>
       </c>
       <c r="C401" t="n">
-        <v>64670</v>
+        <v>63174</v>
       </c>
       <c r="D401" t="n">
         <v>2</v>
@@ -7921,10 +7921,10 @@
         <v>6221</v>
       </c>
       <c r="C416" t="n">
-        <v>62241</v>
+        <v>42768</v>
       </c>
       <c r="D416" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E416">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame02284_id6221.png", "frame02284_id6221.png")</f>
@@ -8461,10 +8461,10 @@
         <v>6792</v>
       </c>
       <c r="C446" t="n">
-        <v>60171</v>
+        <v>34456</v>
       </c>
       <c r="D446" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E446">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame02425_id6792.png", "frame02425_id6792.png")</f>
@@ -8713,7 +8713,7 @@
         <v>6944</v>
       </c>
       <c r="C460" t="n">
-        <v>38980</v>
+        <v>22270</v>
       </c>
       <c r="D460" t="n">
         <v>1</v>
@@ -11395,7 +11395,7 @@
         <v>9470</v>
       </c>
       <c r="C609" t="n">
-        <v>37575</v>
+        <v>22040</v>
       </c>
       <c r="D609" t="n">
         <v>1</v>
@@ -11575,7 +11575,7 @@
         <v>9596</v>
       </c>
       <c r="C619" t="n">
-        <v>31772</v>
+        <v>19995</v>
       </c>
       <c r="D619" t="n">
         <v>1</v>
@@ -14419,7 +14419,7 @@
         <v>12236</v>
       </c>
       <c r="C777" t="n">
-        <v>53374</v>
+        <v>32035</v>
       </c>
       <c r="D777" t="n">
         <v>1</v>
@@ -14491,7 +14491,7 @@
         <v>12249</v>
       </c>
       <c r="C781" t="n">
-        <v>54332</v>
+        <v>53732</v>
       </c>
       <c r="D781" t="n">
         <v>1</v>
@@ -15013,10 +15013,10 @@
         <v>12779</v>
       </c>
       <c r="C810" t="n">
-        <v>69414</v>
+        <v>58706</v>
       </c>
       <c r="D810" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E810">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame04271_id12779.png", "frame04271_id12779.png")</f>
@@ -15121,10 +15121,10 @@
         <v>12813</v>
       </c>
       <c r="C816" t="n">
-        <v>64184</v>
+        <v>41328</v>
       </c>
       <c r="D816" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E816">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame04303_id12813.png", "frame04303_id12813.png")</f>
@@ -16435,7 +16435,7 @@
         <v>14061</v>
       </c>
       <c r="C889" t="n">
-        <v>31718</v>
+        <v>19028</v>
       </c>
       <c r="D889" t="n">
         <v>1</v>
@@ -16489,7 +16489,7 @@
         <v>14101</v>
       </c>
       <c r="C892" t="n">
-        <v>55856</v>
+        <v>32025</v>
       </c>
       <c r="D892" t="n">
         <v>1</v>
@@ -17353,7 +17353,7 @@
         <v>14745</v>
       </c>
       <c r="C940" t="n">
-        <v>55842</v>
+        <v>30240</v>
       </c>
       <c r="D940" t="n">
         <v>1</v>
@@ -18811,7 +18811,7 @@
         <v>15970</v>
       </c>
       <c r="C1021" t="n">
-        <v>74348</v>
+        <v>72518</v>
       </c>
       <c r="D1021" t="n">
         <v>2</v>
@@ -18829,10 +18829,10 @@
         <v>16012</v>
       </c>
       <c r="C1022" t="n">
-        <v>64939</v>
+        <v>43433</v>
       </c>
       <c r="D1022" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1022">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame05341_id16012.png", "frame05341_id16012.png")</f>
@@ -19279,7 +19279,7 @@
         <v>16473</v>
       </c>
       <c r="C1047" t="n">
-        <v>73143</v>
+        <v>72927</v>
       </c>
       <c r="D1047" t="n">
         <v>2</v>
@@ -22483,7 +22483,7 @@
         <v>19526</v>
       </c>
       <c r="C1225" t="n">
-        <v>74418</v>
+        <v>71604</v>
       </c>
       <c r="D1225" t="n">
         <v>2</v>
@@ -23095,7 +23095,7 @@
         <v>20072</v>
       </c>
       <c r="C1259" t="n">
-        <v>53490</v>
+        <v>35696</v>
       </c>
       <c r="D1259" t="n">
         <v>1</v>
@@ -23959,10 +23959,10 @@
         <v>20800</v>
       </c>
       <c r="C1307" t="n">
-        <v>68896</v>
+        <v>38793</v>
       </c>
       <c r="D1307" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1307">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame06672_id20800.png", "frame06672_id20800.png")</f>
@@ -24265,10 +24265,10 @@
         <v>21046</v>
       </c>
       <c r="C1324" t="n">
-        <v>68887</v>
+        <v>58045</v>
       </c>
       <c r="D1324" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1324">
         <f>HYPERLINK("file:///C:/Users/anye forti/Desktop/2025 FALL/426 COSC/YOLO_TESTING/bbox-snapshots/frame06764_id21046.png", "frame06764_id21046.png")</f>
@@ -24535,7 +24535,7 @@
         <v>21442</v>
       </c>
       <c r="C1339" t="n">
-        <v>43467</v>
+        <v>28542</v>
       </c>
       <c r="D1339" t="n">
         <v>1</v>
@@ -26299,7 +26299,7 @@
         <v>23230</v>
       </c>
       <c r="C1437" t="n">
-        <v>51035</v>
+        <v>28416</v>
       </c>
       <c r="D1437" t="n">
         <v>1</v>
@@ -27004,7 +27004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -27042,815 +27042,463 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>125</v>
+        <v>182</v>
       </c>
       <c r="B3" t="n">
-        <v>158</v>
+        <v>298</v>
       </c>
       <c r="C3" t="n">
-        <v>173</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>173</v>
+        <v>515</v>
       </c>
       <c r="B4" t="n">
-        <v>292</v>
+        <v>1001</v>
       </c>
       <c r="C4" t="n">
-        <v>255</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>182</v>
+        <v>685</v>
       </c>
       <c r="B5" t="n">
-        <v>298</v>
+        <v>1641</v>
       </c>
       <c r="C5" t="n">
-        <v>290</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>515</v>
+        <v>805</v>
       </c>
       <c r="B6" t="n">
-        <v>1001</v>
+        <v>2019</v>
       </c>
       <c r="C6" t="n">
-        <v>1042</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>668</v>
+        <v>1073</v>
       </c>
       <c r="B7" t="n">
-        <v>1585</v>
+        <v>2792</v>
       </c>
       <c r="C7" t="n">
-        <v>1613</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>685</v>
+        <v>1188</v>
       </c>
       <c r="B8" t="n">
-        <v>1641</v>
+        <v>3248</v>
       </c>
       <c r="C8" t="n">
-        <v>1736</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>805</v>
+        <v>1323</v>
       </c>
       <c r="B9" t="n">
-        <v>2019</v>
+        <v>3653</v>
       </c>
       <c r="C9" t="n">
-        <v>2056</v>
+        <v>3694</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>984</v>
+        <v>1352</v>
       </c>
       <c r="B10" t="n">
-        <v>2532</v>
+        <v>3689</v>
       </c>
       <c r="C10" t="n">
-        <v>2472</v>
+        <v>3779</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1073</v>
+        <v>1370</v>
       </c>
       <c r="B11" t="n">
-        <v>2792</v>
+        <v>3750</v>
       </c>
       <c r="C11" t="n">
-        <v>2809</v>
+        <v>3828</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1188</v>
+        <v>1393</v>
       </c>
       <c r="B12" t="n">
-        <v>3248</v>
+        <v>3871</v>
       </c>
       <c r="C12" t="n">
-        <v>3222</v>
+        <v>3784</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1323</v>
+        <v>2225</v>
       </c>
       <c r="B13" t="n">
-        <v>3653</v>
+        <v>6108</v>
       </c>
       <c r="C13" t="n">
-        <v>3694</v>
+        <v>6065</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1352</v>
+        <v>2263</v>
       </c>
       <c r="B14" t="n">
-        <v>3689</v>
+        <v>6111</v>
       </c>
       <c r="C14" t="n">
-        <v>3779</v>
+        <v>6211</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1370</v>
+        <v>2514</v>
       </c>
       <c r="B15" t="n">
-        <v>3750</v>
+        <v>7167</v>
       </c>
       <c r="C15" t="n">
-        <v>3828</v>
+        <v>7041</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1393</v>
+        <v>2831</v>
       </c>
       <c r="B16" t="n">
-        <v>3871</v>
+        <v>8175</v>
       </c>
       <c r="C16" t="n">
-        <v>3784</v>
+        <v>8259</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1558</v>
+        <v>3015</v>
       </c>
       <c r="B17" t="n">
-        <v>4453</v>
+        <v>8835</v>
       </c>
       <c r="C17" t="n">
-        <v>4374</v>
+        <v>8764</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1624</v>
+        <v>3137</v>
       </c>
       <c r="B18" t="n">
-        <v>4633</v>
+        <v>9303</v>
       </c>
       <c r="C18" t="n">
-        <v>4591</v>
+        <v>9376</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1801</v>
+        <v>3195</v>
       </c>
       <c r="B19" t="n">
-        <v>5322</v>
+        <v>9527</v>
       </c>
       <c r="C19" t="n">
-        <v>5300</v>
+        <v>9604</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1842</v>
+        <v>3208</v>
       </c>
       <c r="B20" t="n">
-        <v>5482</v>
+        <v>9530</v>
       </c>
       <c r="C20" t="n">
-        <v>5433</v>
+        <v>9576</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2225</v>
+        <v>3358</v>
       </c>
       <c r="B21" t="n">
-        <v>6108</v>
+        <v>10119</v>
       </c>
       <c r="C21" t="n">
-        <v>6017</v>
+        <v>10042</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2225</v>
+        <v>3541</v>
       </c>
       <c r="B22" t="n">
-        <v>6108</v>
+        <v>10689</v>
       </c>
       <c r="C22" t="n">
-        <v>6065</v>
+        <v>10698</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2263</v>
+        <v>3572</v>
       </c>
       <c r="B23" t="n">
-        <v>6111</v>
+        <v>10817</v>
       </c>
       <c r="C23" t="n">
-        <v>6211</v>
+        <v>10784</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2284</v>
+        <v>3606</v>
       </c>
       <c r="B24" t="n">
-        <v>6221</v>
+        <v>10839</v>
       </c>
       <c r="C24" t="n">
-        <v>6196</v>
+        <v>10891</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2425</v>
+        <v>3671</v>
       </c>
       <c r="B25" t="n">
-        <v>6792</v>
+        <v>10961</v>
       </c>
       <c r="C25" t="n">
-        <v>6675</v>
+        <v>10990</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2496</v>
+        <v>4091</v>
       </c>
       <c r="B26" t="n">
-        <v>6944</v>
+        <v>12063</v>
       </c>
       <c r="C26" t="n">
-        <v>6813</v>
+        <v>12094</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2514</v>
+        <v>4114</v>
       </c>
       <c r="B27" t="n">
-        <v>7167</v>
+        <v>12104</v>
       </c>
       <c r="C27" t="n">
-        <v>7041</v>
+        <v>12230</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2831</v>
+        <v>4445</v>
       </c>
       <c r="B28" t="n">
-        <v>8175</v>
+        <v>13230</v>
       </c>
       <c r="C28" t="n">
-        <v>8259</v>
+        <v>13359</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2842</v>
+        <v>4638</v>
       </c>
       <c r="B29" t="n">
-        <v>8136</v>
+        <v>13783</v>
       </c>
       <c r="C29" t="n">
-        <v>8281</v>
+        <v>13807</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>3015</v>
+        <v>5219</v>
       </c>
       <c r="B30" t="n">
-        <v>8835</v>
+        <v>15588</v>
       </c>
       <c r="C30" t="n">
-        <v>8764</v>
+        <v>15554</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>3137</v>
+        <v>5380</v>
       </c>
       <c r="B31" t="n">
-        <v>9303</v>
+        <v>16175</v>
       </c>
       <c r="C31" t="n">
-        <v>9376</v>
+        <v>16247</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>3186</v>
+        <v>5505</v>
       </c>
       <c r="B32" t="n">
-        <v>9470</v>
+        <v>16540</v>
       </c>
       <c r="C32" t="n">
-        <v>9437</v>
+        <v>16705</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>3195</v>
+        <v>5607</v>
       </c>
       <c r="B33" t="n">
-        <v>9527</v>
+        <v>17121</v>
       </c>
       <c r="C33" t="n">
-        <v>9604</v>
+        <v>17068</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>3208</v>
+        <v>5736</v>
       </c>
       <c r="B34" t="n">
-        <v>9530</v>
+        <v>17421</v>
       </c>
       <c r="C34" t="n">
-        <v>9576</v>
+        <v>17464</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>3214</v>
+        <v>5878</v>
       </c>
       <c r="B35" t="n">
-        <v>9596</v>
+        <v>18037</v>
       </c>
       <c r="C35" t="n">
-        <v>9559</v>
+        <v>18033</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>3358</v>
+        <v>6131</v>
       </c>
       <c r="B36" t="n">
-        <v>10119</v>
+        <v>18815</v>
       </c>
       <c r="C36" t="n">
-        <v>10042</v>
+        <v>18897</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>3541</v>
+        <v>6141</v>
       </c>
       <c r="B37" t="n">
-        <v>10689</v>
+        <v>18940</v>
       </c>
       <c r="C37" t="n">
-        <v>10698</v>
+        <v>18897</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>3572</v>
+        <v>6532</v>
       </c>
       <c r="B38" t="n">
-        <v>10817</v>
+        <v>20346</v>
       </c>
       <c r="C38" t="n">
-        <v>10784</v>
+        <v>20255</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>3606</v>
+        <v>6571</v>
       </c>
       <c r="B39" t="n">
-        <v>10839</v>
+        <v>20553</v>
       </c>
       <c r="C39" t="n">
-        <v>10891</v>
+        <v>20617</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>3671</v>
+        <v>6754</v>
       </c>
       <c r="B40" t="n">
-        <v>10961</v>
+        <v>21246</v>
       </c>
       <c r="C40" t="n">
-        <v>10990</v>
+        <v>21278</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>4091</v>
+        <v>7083</v>
       </c>
       <c r="B41" t="n">
-        <v>12063</v>
+        <v>22461</v>
       </c>
       <c r="C41" t="n">
-        <v>12094</v>
+        <v>22555</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>4114</v>
+        <v>7366</v>
       </c>
       <c r="B42" t="n">
-        <v>12104</v>
+        <v>23489</v>
       </c>
       <c r="C42" t="n">
-        <v>12230</v>
+        <v>23511</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>4117</v>
+        <v>7395</v>
       </c>
       <c r="B43" t="n">
-        <v>12236</v>
+        <v>23573</v>
       </c>
       <c r="C43" t="n">
-        <v>12104</v>
+        <v>23620</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>4131</v>
+        <v>7449</v>
       </c>
       <c r="B44" t="n">
-        <v>12249</v>
+        <v>23810</v>
       </c>
       <c r="C44" t="n">
-        <v>12253</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>4271</v>
-      </c>
-      <c r="B45" t="n">
-        <v>12779</v>
-      </c>
-      <c r="C45" t="n">
-        <v>12693</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>4303</v>
-      </c>
-      <c r="B46" t="n">
-        <v>12813</v>
-      </c>
-      <c r="C46" t="n">
-        <v>12772</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="n">
-        <v>4445</v>
-      </c>
-      <c r="B47" t="n">
-        <v>13230</v>
-      </c>
-      <c r="C47" t="n">
-        <v>13359</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="n">
-        <v>4638</v>
-      </c>
-      <c r="B48" t="n">
-        <v>13783</v>
-      </c>
-      <c r="C48" t="n">
-        <v>13807</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="n">
-        <v>4715</v>
-      </c>
-      <c r="B49" t="n">
-        <v>14061</v>
-      </c>
-      <c r="C49" t="n">
-        <v>14032</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="n">
-        <v>4727</v>
-      </c>
-      <c r="B50" t="n">
-        <v>14101</v>
-      </c>
-      <c r="C50" t="n">
-        <v>14071</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="n">
-        <v>4967</v>
-      </c>
-      <c r="B51" t="n">
-        <v>14715</v>
-      </c>
-      <c r="C51" t="n">
-        <v>14711</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>4980</v>
-      </c>
-      <c r="B52" t="n">
-        <v>14745</v>
-      </c>
-      <c r="C52" t="n">
-        <v>14678</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>5219</v>
-      </c>
-      <c r="B53" t="n">
-        <v>15588</v>
-      </c>
-      <c r="C53" t="n">
-        <v>15554</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>5338</v>
-      </c>
-      <c r="B54" t="n">
-        <v>15970</v>
-      </c>
-      <c r="C54" t="n">
-        <v>16037</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>5341</v>
-      </c>
-      <c r="B55" t="n">
-        <v>16012</v>
-      </c>
-      <c r="C55" t="n">
-        <v>15970</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>5380</v>
-      </c>
-      <c r="B56" t="n">
-        <v>16175</v>
-      </c>
-      <c r="C56" t="n">
-        <v>16247</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>5448</v>
-      </c>
-      <c r="B57" t="n">
-        <v>16473</v>
-      </c>
-      <c r="C57" t="n">
-        <v>16462</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>5505</v>
-      </c>
-      <c r="B58" t="n">
-        <v>16540</v>
-      </c>
-      <c r="C58" t="n">
-        <v>16705</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>5607</v>
-      </c>
-      <c r="B59" t="n">
-        <v>17121</v>
-      </c>
-      <c r="C59" t="n">
-        <v>17068</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>5736</v>
-      </c>
-      <c r="B60" t="n">
-        <v>17421</v>
-      </c>
-      <c r="C60" t="n">
-        <v>17464</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>5878</v>
-      </c>
-      <c r="B61" t="n">
-        <v>18037</v>
-      </c>
-      <c r="C61" t="n">
-        <v>18033</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>6131</v>
-      </c>
-      <c r="B62" t="n">
-        <v>18815</v>
-      </c>
-      <c r="C62" t="n">
-        <v>18897</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>6141</v>
-      </c>
-      <c r="B63" t="n">
-        <v>18940</v>
-      </c>
-      <c r="C63" t="n">
-        <v>18897</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>6335</v>
-      </c>
-      <c r="B64" t="n">
-        <v>19526</v>
-      </c>
-      <c r="C64" t="n">
-        <v>19414</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>6480</v>
-      </c>
-      <c r="B65" t="n">
-        <v>20072</v>
-      </c>
-      <c r="C65" t="n">
-        <v>20108</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>6532</v>
-      </c>
-      <c r="B66" t="n">
-        <v>20346</v>
-      </c>
-      <c r="C66" t="n">
-        <v>20255</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n">
-        <v>6571</v>
-      </c>
-      <c r="B67" t="n">
-        <v>20553</v>
-      </c>
-      <c r="C67" t="n">
-        <v>20617</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="n">
-        <v>6672</v>
-      </c>
-      <c r="B68" t="n">
-        <v>20800</v>
-      </c>
-      <c r="C68" t="n">
-        <v>20906</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="n">
-        <v>6754</v>
-      </c>
-      <c r="B69" t="n">
-        <v>21246</v>
-      </c>
-      <c r="C69" t="n">
-        <v>21278</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="n">
-        <v>6764</v>
-      </c>
-      <c r="B70" t="n">
-        <v>21046</v>
-      </c>
-      <c r="C70" t="n">
-        <v>21246</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n">
-        <v>6809</v>
-      </c>
-      <c r="B71" t="n">
-        <v>21442</v>
-      </c>
-      <c r="C71" t="n">
-        <v>21456</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="n">
-        <v>7083</v>
-      </c>
-      <c r="B72" t="n">
-        <v>22461</v>
-      </c>
-      <c r="C72" t="n">
-        <v>22555</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="n">
-        <v>7279</v>
-      </c>
-      <c r="B73" t="n">
-        <v>23230</v>
-      </c>
-      <c r="C73" t="n">
-        <v>23269</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="n">
-        <v>7366</v>
-      </c>
-      <c r="B74" t="n">
-        <v>23489</v>
-      </c>
-      <c r="C74" t="n">
-        <v>23511</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="n">
-        <v>7395</v>
-      </c>
-      <c r="B75" t="n">
-        <v>23573</v>
-      </c>
-      <c r="C75" t="n">
-        <v>23620</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="n">
-        <v>7449</v>
-      </c>
-      <c r="B76" t="n">
-        <v>23810</v>
-      </c>
-      <c r="C76" t="n">
         <v>23743</v>
       </c>
     </row>

</xml_diff>